<commit_message>
another major milestone - scaleable units implemented mimicing BeerJSON format
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Brewing\Software\RecipePlanner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C98C0E37-C62E-48B6-94CB-01C80C6252C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E739E141-75C1-42EB-A9B8-D92D0FDF96CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{CDF466C7-5B50-42D7-8D0F-5D6B49FA8285}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{CDF466C7-5B50-42D7-8D0F-5D6B49FA8285}"/>
   </bookViews>
   <sheets>
     <sheet name="Styles" sheetId="5" r:id="rId1"/>
@@ -4047,28 +4047,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4087,6 +4066,27 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4433,61 +4433,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="39" t="s">
         <v>203</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="39" t="s">
         <v>204</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="39" t="s">
         <v>1009</v>
       </c>
-      <c r="D1" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="35"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="37" t="s">
+      <c r="D1" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="31"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="43" t="s">
         <v>1010</v>
       </c>
-      <c r="H1" s="38"/>
-      <c r="I1" s="31" t="s">
+      <c r="H1" s="44"/>
+      <c r="I1" s="38" t="s">
         <v>1011</v>
       </c>
-      <c r="J1" s="31"/>
-      <c r="K1" s="40" t="s">
+      <c r="J1" s="38"/>
+      <c r="K1" s="33" t="s">
         <v>1012</v>
       </c>
-      <c r="L1" s="41"/>
-      <c r="M1" s="42" t="s">
+      <c r="L1" s="34"/>
+      <c r="M1" s="35" t="s">
         <v>1013</v>
       </c>
-      <c r="N1" s="42"/>
-      <c r="O1" s="43" t="s">
+      <c r="N1" s="35"/>
+      <c r="O1" s="36" t="s">
         <v>1014</v>
       </c>
-      <c r="P1" s="44"/>
-      <c r="Q1" s="43" t="s">
+      <c r="P1" s="37"/>
+      <c r="Q1" s="36" t="s">
         <v>1015</v>
       </c>
-      <c r="R1" s="44"/>
-      <c r="S1" s="35" t="s">
+      <c r="R1" s="37"/>
+      <c r="S1" s="31" t="s">
         <v>223</v>
       </c>
-      <c r="T1" s="35" t="s">
+      <c r="T1" s="31" t="s">
         <v>1004</v>
       </c>
-      <c r="U1" s="35" t="s">
+      <c r="U1" s="31" t="s">
         <v>1003</v>
       </c>
-      <c r="V1" s="35" t="s">
+      <c r="V1" s="31" t="s">
         <v>1002</v>
       </c>
     </row>
     <row r="2" spans="1:22" s="15" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="33"/>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
+      <c r="A2" s="40"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
       <c r="D2" s="24" t="s">
         <v>1005</v>
       </c>
@@ -4533,10 +4533,10 @@
       <c r="R2" s="17" t="s">
         <v>1017</v>
       </c>
-      <c r="S2" s="39"/>
-      <c r="T2" s="39"/>
-      <c r="U2" s="39"/>
-      <c r="V2" s="39"/>
+      <c r="S2" s="32"/>
+      <c r="T2" s="32"/>
+      <c r="U2" s="32"/>
+      <c r="V2" s="32"/>
     </row>
     <row r="3" spans="1:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -11152,6 +11152,12 @@
     </sortState>
   </autoFilter>
   <mergeCells count="14">
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="G1:H1"/>
     <mergeCell ref="U1:U2"/>
     <mergeCell ref="V1:V2"/>
     <mergeCell ref="K1:L1"/>
@@ -11160,12 +11166,6 @@
     <mergeCell ref="Q1:R1"/>
     <mergeCell ref="S1:S2"/>
     <mergeCell ref="T1:T2"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="G1:H1"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B1048576" xr:uid="{A6DCB9C4-B06B-4870-87D5-BA96103BC11D}">

</xml_diff>

<commit_message>
added attenuation into cultures and calculations
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Brewing\Software\RecipePlanner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E739E141-75C1-42EB-A9B8-D92D0FDF96CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82118FD9-E7B7-4843-B5FF-00A6F3B64D00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{CDF466C7-5B50-42D7-8D0F-5D6B49FA8285}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{CDF466C7-5B50-42D7-8D0F-5D6B49FA8285}"/>
   </bookViews>
   <sheets>
     <sheet name="Styles" sheetId="5" r:id="rId1"/>
@@ -4047,7 +4047,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4066,27 +4087,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4433,61 +4433,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="32" t="s">
         <v>203</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="32" t="s">
         <v>204</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="32" t="s">
         <v>1009</v>
       </c>
-      <c r="D1" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="31"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="43" t="s">
+      <c r="D1" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="35"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="37" t="s">
         <v>1010</v>
       </c>
-      <c r="H1" s="44"/>
-      <c r="I1" s="38" t="s">
+      <c r="H1" s="38"/>
+      <c r="I1" s="31" t="s">
         <v>1011</v>
       </c>
-      <c r="J1" s="38"/>
-      <c r="K1" s="33" t="s">
+      <c r="J1" s="31"/>
+      <c r="K1" s="40" t="s">
         <v>1012</v>
       </c>
-      <c r="L1" s="34"/>
-      <c r="M1" s="35" t="s">
+      <c r="L1" s="41"/>
+      <c r="M1" s="42" t="s">
         <v>1013</v>
       </c>
-      <c r="N1" s="35"/>
-      <c r="O1" s="36" t="s">
+      <c r="N1" s="42"/>
+      <c r="O1" s="43" t="s">
         <v>1014</v>
       </c>
-      <c r="P1" s="37"/>
-      <c r="Q1" s="36" t="s">
+      <c r="P1" s="44"/>
+      <c r="Q1" s="43" t="s">
         <v>1015</v>
       </c>
-      <c r="R1" s="37"/>
-      <c r="S1" s="31" t="s">
+      <c r="R1" s="44"/>
+      <c r="S1" s="35" t="s">
         <v>223</v>
       </c>
-      <c r="T1" s="31" t="s">
+      <c r="T1" s="35" t="s">
         <v>1004</v>
       </c>
-      <c r="U1" s="31" t="s">
+      <c r="U1" s="35" t="s">
         <v>1003</v>
       </c>
-      <c r="V1" s="31" t="s">
+      <c r="V1" s="35" t="s">
         <v>1002</v>
       </c>
     </row>
     <row r="2" spans="1:22" s="15" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="40"/>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
+      <c r="A2" s="33"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
       <c r="D2" s="24" t="s">
         <v>1005</v>
       </c>
@@ -4533,10 +4533,10 @@
       <c r="R2" s="17" t="s">
         <v>1017</v>
       </c>
-      <c r="S2" s="32"/>
-      <c r="T2" s="32"/>
-      <c r="U2" s="32"/>
-      <c r="V2" s="32"/>
+      <c r="S2" s="39"/>
+      <c r="T2" s="39"/>
+      <c r="U2" s="39"/>
+      <c r="V2" s="39"/>
     </row>
     <row r="3" spans="1:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -11152,12 +11152,6 @@
     </sortState>
   </autoFilter>
   <mergeCells count="14">
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="G1:H1"/>
     <mergeCell ref="U1:U2"/>
     <mergeCell ref="V1:V2"/>
     <mergeCell ref="K1:L1"/>
@@ -11166,6 +11160,12 @@
     <mergeCell ref="Q1:R1"/>
     <mergeCell ref="S1:S2"/>
     <mergeCell ref="T1:T2"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="G1:H1"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B1048576" xr:uid="{A6DCB9C4-B06B-4870-87D5-BA96103BC11D}">
@@ -20717,7 +20717,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C200754A-849E-424D-9967-CE80DF2DBB8D}">
   <dimension ref="A1:M64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
@@ -23355,11 +23355,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2F56AC2-CB84-477F-887D-0F7013E70CB1}">
   <dimension ref="A1:N124"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B62" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F69" sqref="F69"/>
+      <selection pane="bottomRight" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23439,6 +23439,9 @@
       <c r="F2" s="29">
         <v>0.8</v>
       </c>
+      <c r="G2" s="29">
+        <v>0.9</v>
+      </c>
       <c r="I2" t="s">
         <v>1021</v>
       </c>
@@ -23468,6 +23471,9 @@
       <c r="F3" s="29">
         <v>0.7</v>
       </c>
+      <c r="G3" s="29">
+        <v>0.7</v>
+      </c>
       <c r="I3" t="s">
         <v>1021</v>
       </c>
@@ -23497,6 +23503,9 @@
       <c r="F4" s="29">
         <v>0.75</v>
       </c>
+      <c r="G4" s="29">
+        <v>0.75</v>
+      </c>
       <c r="I4" t="s">
         <v>1021</v>
       </c>
@@ -23524,6 +23533,9 @@
         <v>1024</v>
       </c>
       <c r="F5" s="29">
+        <v>0.75</v>
+      </c>
+      <c r="G5" s="29">
         <v>0.75</v>
       </c>
       <c r="I5" t="s">

</xml_diff>

<commit_message>
began adding support for brewing salts (still broken) but fixed mash step calculations for temp and volume
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -8,21 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Brewing\Software\RecipePlanner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82118FD9-E7B7-4843-B5FF-00A6F3B64D00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B217C6FC-6A0C-49EC-A45C-ACC0FDED8E08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{CDF466C7-5B50-42D7-8D0F-5D6B49FA8285}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{CDF466C7-5B50-42D7-8D0F-5D6B49FA8285}"/>
   </bookViews>
   <sheets>
     <sheet name="Styles" sheetId="5" r:id="rId1"/>
     <sheet name="Fermentables" sheetId="3" r:id="rId2"/>
     <sheet name="Hops" sheetId="4" r:id="rId3"/>
     <sheet name="Cultures" sheetId="6" r:id="rId4"/>
+    <sheet name="Waters" sheetId="7" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Cultures!$A$1:$N$124</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Fermentables!$A$1:$O$212</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Hops!$A$1:$M$64</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Styles!$A$2:$V$100</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Waters!$A$1:$I$3</definedName>
   </definedNames>
   <calcPr calcId="191029" iterate="1" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3141" uniqueCount="1278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3154" uniqueCount="1289">
   <si>
     <t>Style</t>
   </si>
@@ -3876,6 +3878,39 @@
   </si>
   <si>
     <t>Typically used for making rice wine but has shown to ferment beer just fine. The ester profile is very fruity and produces a surprising amount of alcohol (15%). The aroma and flavor were highly favorable compared to rice wine made with the traditional yeast balls.</t>
+  </si>
+  <si>
+    <t>Calcium</t>
+  </si>
+  <si>
+    <t>Magnesium</t>
+  </si>
+  <si>
+    <t>Sodium</t>
+  </si>
+  <si>
+    <t>Chloride</t>
+  </si>
+  <si>
+    <t>Sulfate</t>
+  </si>
+  <si>
+    <t>Bicarbonate</t>
+  </si>
+  <si>
+    <t>pH</t>
+  </si>
+  <si>
+    <t>Distilled</t>
+  </si>
+  <si>
+    <t>Bay City</t>
+  </si>
+  <si>
+    <t>Generic entry for distilled water purchased from the store.</t>
+  </si>
+  <si>
+    <t>From a report from Ward Laboratories commissioned on 3/31/2020.</t>
   </si>
 </sst>
 </file>
@@ -4047,28 +4082,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4087,6 +4101,27 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4433,61 +4468,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="39" t="s">
         <v>203</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="39" t="s">
         <v>204</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="39" t="s">
         <v>1009</v>
       </c>
-      <c r="D1" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="35"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="37" t="s">
+      <c r="D1" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="31"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="43" t="s">
         <v>1010</v>
       </c>
-      <c r="H1" s="38"/>
-      <c r="I1" s="31" t="s">
+      <c r="H1" s="44"/>
+      <c r="I1" s="38" t="s">
         <v>1011</v>
       </c>
-      <c r="J1" s="31"/>
-      <c r="K1" s="40" t="s">
+      <c r="J1" s="38"/>
+      <c r="K1" s="33" t="s">
         <v>1012</v>
       </c>
-      <c r="L1" s="41"/>
-      <c r="M1" s="42" t="s">
+      <c r="L1" s="34"/>
+      <c r="M1" s="35" t="s">
         <v>1013</v>
       </c>
-      <c r="N1" s="42"/>
-      <c r="O1" s="43" t="s">
+      <c r="N1" s="35"/>
+      <c r="O1" s="36" t="s">
         <v>1014</v>
       </c>
-      <c r="P1" s="44"/>
-      <c r="Q1" s="43" t="s">
+      <c r="P1" s="37"/>
+      <c r="Q1" s="36" t="s">
         <v>1015</v>
       </c>
-      <c r="R1" s="44"/>
-      <c r="S1" s="35" t="s">
+      <c r="R1" s="37"/>
+      <c r="S1" s="31" t="s">
         <v>223</v>
       </c>
-      <c r="T1" s="35" t="s">
+      <c r="T1" s="31" t="s">
         <v>1004</v>
       </c>
-      <c r="U1" s="35" t="s">
+      <c r="U1" s="31" t="s">
         <v>1003</v>
       </c>
-      <c r="V1" s="35" t="s">
+      <c r="V1" s="31" t="s">
         <v>1002</v>
       </c>
     </row>
     <row r="2" spans="1:22" s="15" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="33"/>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
+      <c r="A2" s="40"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
       <c r="D2" s="24" t="s">
         <v>1005</v>
       </c>
@@ -4533,10 +4568,10 @@
       <c r="R2" s="17" t="s">
         <v>1017</v>
       </c>
-      <c r="S2" s="39"/>
-      <c r="T2" s="39"/>
-      <c r="U2" s="39"/>
-      <c r="V2" s="39"/>
+      <c r="S2" s="32"/>
+      <c r="T2" s="32"/>
+      <c r="U2" s="32"/>
+      <c r="V2" s="32"/>
     </row>
     <row r="3" spans="1:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -11152,6 +11187,12 @@
     </sortState>
   </autoFilter>
   <mergeCells count="14">
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="G1:H1"/>
     <mergeCell ref="U1:U2"/>
     <mergeCell ref="V1:V2"/>
     <mergeCell ref="K1:L1"/>
@@ -11160,12 +11201,6 @@
     <mergeCell ref="Q1:R1"/>
     <mergeCell ref="S1:S2"/>
     <mergeCell ref="T1:T2"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="G1:H1"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B1048576" xr:uid="{A6DCB9C4-B06B-4870-87D5-BA96103BC11D}">
@@ -23355,7 +23390,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2F56AC2-CB84-477F-887D-0F7013E70CB1}">
   <dimension ref="A1:N124"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -28241,4 +28276,122 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C28D1FEB-4166-4FC4-8871-127B51015D85}">
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="93.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1278</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>1279</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>1280</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>1281</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>1282</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>1283</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>1284</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1286</v>
+      </c>
+      <c r="B2">
+        <v>33.4</v>
+      </c>
+      <c r="C2">
+        <v>8</v>
+      </c>
+      <c r="D2">
+        <v>7</v>
+      </c>
+      <c r="E2">
+        <v>11</v>
+      </c>
+      <c r="F2">
+        <v>6</v>
+      </c>
+      <c r="G2">
+        <v>107</v>
+      </c>
+      <c r="H2">
+        <v>7.9</v>
+      </c>
+      <c r="I2" t="s">
+        <v>1288</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1285</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>7</v>
+      </c>
+      <c r="I3" t="s">
+        <v>1287</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:I3" xr:uid="{AE6419A9-73C7-4898-84AF-BAB225F6E0B4}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I3">
+      <sortCondition ref="A1:A3"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
major overhaul of the waters tab to limit to just two waters (source and distilled), greatly simplifying other maths
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Brewing\Software\RecipePlanner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B217C6FC-6A0C-49EC-A45C-ACC0FDED8E08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F5CF845-56FD-4353-A1EA-33FB4542ED4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{CDF466C7-5B50-42D7-8D0F-5D6B49FA8285}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3154" uniqueCount="1289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3152" uniqueCount="1287">
   <si>
     <t>Style</t>
   </si>
@@ -3901,13 +3901,7 @@
     <t>pH</t>
   </si>
   <si>
-    <t>Distilled</t>
-  </si>
-  <si>
     <t>Bay City</t>
-  </si>
-  <si>
-    <t>Generic entry for distilled water purchased from the store.</t>
   </si>
   <si>
     <t>From a report from Ward Laboratories commissioned on 3/31/2020.</t>
@@ -4082,7 +4076,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4101,27 +4116,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4468,61 +4462,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="32" t="s">
         <v>203</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="32" t="s">
         <v>204</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="32" t="s">
         <v>1009</v>
       </c>
-      <c r="D1" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="31"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="43" t="s">
+      <c r="D1" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="35"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="37" t="s">
         <v>1010</v>
       </c>
-      <c r="H1" s="44"/>
-      <c r="I1" s="38" t="s">
+      <c r="H1" s="38"/>
+      <c r="I1" s="31" t="s">
         <v>1011</v>
       </c>
-      <c r="J1" s="38"/>
-      <c r="K1" s="33" t="s">
+      <c r="J1" s="31"/>
+      <c r="K1" s="40" t="s">
         <v>1012</v>
       </c>
-      <c r="L1" s="34"/>
-      <c r="M1" s="35" t="s">
+      <c r="L1" s="41"/>
+      <c r="M1" s="42" t="s">
         <v>1013</v>
       </c>
-      <c r="N1" s="35"/>
-      <c r="O1" s="36" t="s">
+      <c r="N1" s="42"/>
+      <c r="O1" s="43" t="s">
         <v>1014</v>
       </c>
-      <c r="P1" s="37"/>
-      <c r="Q1" s="36" t="s">
+      <c r="P1" s="44"/>
+      <c r="Q1" s="43" t="s">
         <v>1015</v>
       </c>
-      <c r="R1" s="37"/>
-      <c r="S1" s="31" t="s">
+      <c r="R1" s="44"/>
+      <c r="S1" s="35" t="s">
         <v>223</v>
       </c>
-      <c r="T1" s="31" t="s">
+      <c r="T1" s="35" t="s">
         <v>1004</v>
       </c>
-      <c r="U1" s="31" t="s">
+      <c r="U1" s="35" t="s">
         <v>1003</v>
       </c>
-      <c r="V1" s="31" t="s">
+      <c r="V1" s="35" t="s">
         <v>1002</v>
       </c>
     </row>
     <row r="2" spans="1:22" s="15" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="40"/>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
+      <c r="A2" s="33"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
       <c r="D2" s="24" t="s">
         <v>1005</v>
       </c>
@@ -4568,10 +4562,10 @@
       <c r="R2" s="17" t="s">
         <v>1017</v>
       </c>
-      <c r="S2" s="32"/>
-      <c r="T2" s="32"/>
-      <c r="U2" s="32"/>
-      <c r="V2" s="32"/>
+      <c r="S2" s="39"/>
+      <c r="T2" s="39"/>
+      <c r="U2" s="39"/>
+      <c r="V2" s="39"/>
     </row>
     <row r="3" spans="1:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -11187,12 +11181,6 @@
     </sortState>
   </autoFilter>
   <mergeCells count="14">
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="G1:H1"/>
     <mergeCell ref="U1:U2"/>
     <mergeCell ref="V1:V2"/>
     <mergeCell ref="K1:L1"/>
@@ -11201,6 +11189,12 @@
     <mergeCell ref="Q1:R1"/>
     <mergeCell ref="S1:S2"/>
     <mergeCell ref="T1:T2"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="G1:H1"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B1048576" xr:uid="{A6DCB9C4-B06B-4870-87D5-BA96103BC11D}">
@@ -28280,10 +28274,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C28D1FEB-4166-4FC4-8871-127B51015D85}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28330,7 +28324,7 @@
     </row>
     <row r="2" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="B2">
         <v>33.4</v>
@@ -28354,36 +28348,7 @@
         <v>7.9</v>
       </c>
       <c r="I2" t="s">
-        <v>1288</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1285</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>7</v>
-      </c>
-      <c r="I3" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed from pipenv to poetry for dependency management
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Brewing\Software\AlphaBrew\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Projects\Brewing\Software\AlphaBrew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA14D8EF-2B07-42DB-BA35-B27F3AC6BA8C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7620A010-867C-48A4-8FBD-CD18788B8758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CDF466C7-5B50-42D7-8D0F-5D6B49FA8285}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{CDF466C7-5B50-42D7-8D0F-5D6B49FA8285}"/>
   </bookViews>
   <sheets>
     <sheet name="Styles" sheetId="5" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3130" uniqueCount="1258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3136" uniqueCount="1261">
   <si>
     <t>Style</t>
   </si>
@@ -3818,6 +3818,15 @@
   </si>
   <si>
     <t>Black IPA</t>
+  </si>
+  <si>
+    <t>Cara 8 Malt</t>
+  </si>
+  <si>
+    <t>Dingemans</t>
+  </si>
+  <si>
+    <t>Adding this type of malt increases the foam stability of your beers. Trough it’s light colour it can even be added in low percentages in your Pilsen beer to improve the foam stability.</t>
   </si>
 </sst>
 </file>
@@ -3999,7 +4008,28 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4018,27 +4048,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4359,7 +4368,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DD9F28D-7B72-455D-AE84-5081F2A35C92}">
   <dimension ref="A1:V101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="S21" sqref="S21"/>
     </sheetView>
   </sheetViews>
@@ -4385,61 +4394,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="34" t="s">
         <v>179</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="34" t="s">
         <v>180</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="34" t="s">
         <v>957</v>
       </c>
-      <c r="D1" s="43" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="33"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="45" t="s">
+      <c r="D1" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="37"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="39" t="s">
         <v>958</v>
       </c>
-      <c r="H1" s="46"/>
-      <c r="I1" s="40" t="s">
+      <c r="H1" s="40"/>
+      <c r="I1" s="33" t="s">
         <v>959</v>
       </c>
-      <c r="J1" s="40"/>
-      <c r="K1" s="35" t="s">
+      <c r="J1" s="33"/>
+      <c r="K1" s="42" t="s">
         <v>960</v>
       </c>
-      <c r="L1" s="36"/>
-      <c r="M1" s="37" t="s">
+      <c r="L1" s="43"/>
+      <c r="M1" s="44" t="s">
         <v>961</v>
       </c>
-      <c r="N1" s="37"/>
-      <c r="O1" s="38" t="s">
+      <c r="N1" s="44"/>
+      <c r="O1" s="45" t="s">
         <v>962</v>
       </c>
-      <c r="P1" s="39"/>
-      <c r="Q1" s="38" t="s">
+      <c r="P1" s="46"/>
+      <c r="Q1" s="45" t="s">
         <v>963</v>
       </c>
-      <c r="R1" s="39"/>
-      <c r="S1" s="33" t="s">
+      <c r="R1" s="46"/>
+      <c r="S1" s="37" t="s">
         <v>196</v>
       </c>
-      <c r="T1" s="33" t="s">
+      <c r="T1" s="37" t="s">
         <v>952</v>
       </c>
-      <c r="U1" s="33" t="s">
+      <c r="U1" s="37" t="s">
         <v>951</v>
       </c>
-      <c r="V1" s="33" t="s">
+      <c r="V1" s="37" t="s">
         <v>950</v>
       </c>
     </row>
     <row r="2" spans="1:22" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="42"/>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
+      <c r="A2" s="35"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
       <c r="D2" s="22" t="s">
         <v>953</v>
       </c>
@@ -4485,10 +4494,10 @@
       <c r="R2" s="15" t="s">
         <v>965</v>
       </c>
-      <c r="S2" s="34"/>
-      <c r="T2" s="34"/>
-      <c r="U2" s="34"/>
-      <c r="V2" s="34"/>
+      <c r="S2" s="41"/>
+      <c r="T2" s="41"/>
+      <c r="U2" s="41"/>
+      <c r="V2" s="41"/>
     </row>
     <row r="3" spans="1:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -11160,12 +11169,6 @@
     </sortState>
   </autoFilter>
   <mergeCells count="14">
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="G1:H1"/>
     <mergeCell ref="U1:U2"/>
     <mergeCell ref="V1:V2"/>
     <mergeCell ref="K1:L1"/>
@@ -11174,6 +11177,12 @@
     <mergeCell ref="Q1:R1"/>
     <mergeCell ref="S1:S2"/>
     <mergeCell ref="T1:T2"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="G1:H1"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B1048576" xr:uid="{A6DCB9C4-B06B-4870-87D5-BA96103BC11D}">
@@ -11188,13 +11197,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{376299B9-AA91-42AA-B33D-63AEAA70426D}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:N208"/>
+  <dimension ref="A1:N209"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B153" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="N183" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A144" sqref="A144"/>
+      <selection pane="bottomRight" activeCell="N206" sqref="N206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19063,6 +19072,44 @@
       </c>
       <c r="K208" t="b">
         <v>1</v>
+      </c>
+    </row>
+    <row r="209" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>1258</v>
+      </c>
+      <c r="B209" t="s">
+        <v>36</v>
+      </c>
+      <c r="C209" t="s">
+        <v>189</v>
+      </c>
+      <c r="D209" t="s">
+        <v>1259</v>
+      </c>
+      <c r="E209" t="s">
+        <v>57</v>
+      </c>
+      <c r="F209" s="3">
+        <v>75</v>
+      </c>
+      <c r="G209" s="32">
+        <v>8</v>
+      </c>
+      <c r="H209" s="4">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="I209" s="2">
+        <v>0</v>
+      </c>
+      <c r="J209" t="b">
+        <v>0</v>
+      </c>
+      <c r="K209" t="b">
+        <v>1</v>
+      </c>
+      <c r="N209" t="s">
+        <v>1260</v>
       </c>
     </row>
   </sheetData>

</xml_diff>